<commit_message>
navie_bayes - kmeans - desition tree
</commit_message>
<xml_diff>
--- a/uploads/input_bayes_laplaces.xlsx
+++ b/uploads/input_bayes_laplaces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KTDL\BTTH5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB8F073-FAFC-4C74-A70A-074E0403F406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67424259-8BEB-4BD9-BB6D-B5B2A7D77B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{02730827-7C81-4539-827E-22283D60E1E2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10800" xr2:uid="{02730827-7C81-4539-827E-22283D60E1E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -125,13 +125,13 @@
     <t>Temperature</t>
   </si>
   <si>
-    <t xml:space="preserve"> Humidity</t>
-  </si>
-  <si>
     <t>Wind</t>
   </si>
   <si>
     <t>Play ball</t>
+  </si>
+  <si>
+    <t>Humidity</t>
   </si>
 </sst>
 </file>
@@ -212,12 +212,12 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,10 +555,14 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="14.90625" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -571,13 +575,13 @@
         <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>